<commit_message>
update data & code
</commit_message>
<xml_diff>
--- a/result/result3.xlsx
+++ b/result/result3.xlsx
@@ -169,9 +169,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -211,22 +211,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -241,38 +240,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -288,17 +272,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -311,14 +295,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -339,18 +331,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -385,13 +385,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,13 +403,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,37 +517,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,25 +535,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,61 +547,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,28 +617,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -652,17 +632,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -682,6 +658,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -693,6 +678,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -716,94 +716,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -812,56 +812,56 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -890,9 +890,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
@@ -1284,7 +1281,7 @@
       <c r="B3" s="6">
         <v>0</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>0</v>
       </c>
       <c r="D3" s="7">
@@ -1296,14 +1293,14 @@
       <c r="F3" s="9">
         <v>-0.0304125</v>
       </c>
-      <c r="G3" s="10">
-        <v>5.42101e-20</v>
-      </c>
-      <c r="H3" s="10">
-        <v>-2.69433e-19</v>
-      </c>
-      <c r="I3" s="10">
-        <v>-1.05879e-21</v>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:9">
@@ -1583,7 +1580,7 @@
       <c r="E13" s="8">
         <v>0.384608591</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <v>-0.294178533</v>
       </c>
       <c r="G13" s="6">
@@ -1612,7 +1609,7 @@
       <c r="E14" s="8">
         <v>0.481803421</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <v>-0.299784775</v>
       </c>
       <c r="G14" s="6">
@@ -1641,7 +1638,7 @@
       <c r="E15" s="8">
         <v>0.580873302</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="10">
         <v>-0.302884094</v>
       </c>
       <c r="G15" s="6">
@@ -1670,7 +1667,7 @@
       <c r="E16" s="8">
         <v>0.65636512</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <v>-0.300106986</v>
       </c>
       <c r="G16" s="6">
@@ -1699,7 +1696,7 @@
       <c r="E17" s="8">
         <v>0.673523422</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <v>-0.288043662</v>
       </c>
       <c r="G17" s="6">
@@ -1728,7 +1725,7 @@
       <c r="E18" s="8">
         <v>0.608680988</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <v>-0.263147696</v>
       </c>
       <c r="G18" s="6">
@@ -1757,7 +1754,7 @@
       <c r="E19" s="8">
         <v>0.466047241</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <v>-0.22336982</v>
       </c>
       <c r="G19" s="6">
@@ -1786,7 +1783,7 @@
       <c r="E20" s="8">
         <v>0.279115549</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="10">
         <v>-0.17244585</v>
       </c>
       <c r="G20" s="6">
@@ -1815,7 +1812,7 @@
       <c r="E21" s="8">
         <v>0.089689327</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="10">
         <v>-0.121185537</v>
       </c>
       <c r="G21" s="6">
@@ -1844,7 +1841,7 @@
       <c r="E22" s="8">
         <v>-0.08140286</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="10">
         <v>-0.08350758</v>
       </c>
       <c r="G22" s="6">
@@ -1873,7 +1870,7 @@
       <c r="E23" s="8">
         <v>-0.233878814</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="10">
         <v>-0.069420147</v>
       </c>
       <c r="G23" s="6">
@@ -1902,7 +1899,7 @@
       <c r="E24" s="8">
         <v>-0.368837157</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="10">
         <v>-0.081524104</v>
       </c>
       <c r="G24" s="6">
@@ -1931,7 +1928,7 @@
       <c r="E25" s="8">
         <v>-0.478795153</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <v>-0.116052599</v>
       </c>
       <c r="G25" s="6">
@@ -1960,7 +1957,7 @@
       <c r="E26" s="8">
         <v>-0.549281481</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="10">
         <v>-0.165365549</v>
       </c>
       <c r="G26" s="6">
@@ -1989,7 +1986,7 @@
       <c r="E27" s="8">
         <v>-0.565606099</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="10">
         <v>-0.219387017</v>
       </c>
       <c r="G27" s="6">
@@ -2018,7 +2015,7 @@
       <c r="E28" s="8">
         <v>-0.526068661</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="10">
         <v>-0.267967434</v>
       </c>
       <c r="G28" s="6">
@@ -2047,7 +2044,7 @@
       <c r="E29" s="8">
         <v>-0.442109147</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="10">
         <v>-0.304998345</v>
       </c>
       <c r="G29" s="6">
@@ -2076,7 +2073,7 @@
       <c r="E30" s="8">
         <v>-0.331092146</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="10">
         <v>-0.32921939</v>
       </c>
       <c r="G30" s="6">
@@ -2105,7 +2102,7 @@
       <c r="E31" s="8">
         <v>-0.210754697</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="10">
         <v>-0.342209999</v>
       </c>
       <c r="G31" s="6">
@@ -2134,7 +2131,7 @@
       <c r="E32" s="8">
         <v>-0.089294958</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="10">
         <v>-0.345242955</v>
       </c>
       <c r="G32" s="6">
@@ -2163,7 +2160,7 @@
       <c r="E33" s="8">
         <v>0.029639011</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="10">
         <v>-0.338983382</v>
       </c>
       <c r="G33" s="6">
@@ -2192,7 +2189,7 @@
       <c r="E34" s="8">
         <v>0.147713284</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="10">
         <v>-0.324306966</v>
       </c>
       <c r="G34" s="6">
@@ -2221,7 +2218,7 @@
       <c r="E35" s="8">
         <v>0.262993487</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="10">
         <v>-0.302958306</v>
       </c>
       <c r="G35" s="6">
@@ -2250,7 +2247,7 @@
       <c r="E36" s="8">
         <v>0.371452818</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="10">
         <v>-0.27714132</v>
       </c>
       <c r="G36" s="6">
@@ -2279,7 +2276,7 @@
       <c r="E37" s="8">
         <v>0.462130039</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="10">
         <v>-0.249112527</v>
       </c>
       <c r="G37" s="6">
@@ -2308,7 +2305,7 @@
       <c r="E38" s="8">
         <v>0.52283601</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F38" s="10">
         <v>-0.220784193</v>
       </c>
       <c r="G38" s="6">
@@ -2337,7 +2334,7 @@
       <c r="E39" s="8">
         <v>0.541325331</v>
       </c>
-      <c r="F39" s="11">
+      <c r="F39" s="10">
         <v>-0.193810139</v>
       </c>
       <c r="G39" s="6">
@@ -2366,7 +2363,7 @@
       <c r="E40" s="8">
         <v>0.510412996</v>
       </c>
-      <c r="F40" s="11">
+      <c r="F40" s="10">
         <v>-0.169888098</v>
       </c>
       <c r="G40" s="6">
@@ -2395,7 +2392,7 @@
       <c r="E41" s="8">
         <v>0.427442378</v>
       </c>
-      <c r="F41" s="11">
+      <c r="F41" s="10">
         <v>-0.150972079</v>
       </c>
       <c r="G41" s="6">
@@ -2424,7 +2421,7 @@
       <c r="E42" s="8">
         <v>0.292470848</v>
       </c>
-      <c r="F42" s="11">
+      <c r="F42" s="10">
         <v>-0.139288657</v>
       </c>
       <c r="G42" s="6">
@@ -2453,7 +2450,7 @@
       <c r="E43" s="8">
         <v>0.110764085</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F43" s="10">
         <v>-0.136451993</v>
       </c>
       <c r="G43" s="6">
@@ -2482,7 +2479,7 @@
       <c r="E44" s="8">
         <v>-0.100939497</v>
       </c>
-      <c r="F44" s="11">
+      <c r="F44" s="10">
         <v>-0.142820521</v>
       </c>
       <c r="G44" s="6">
@@ -2511,7 +2508,7 @@
       <c r="E45" s="8">
         <v>-0.31054829</v>
       </c>
-      <c r="F45" s="11">
+      <c r="F45" s="10">
         <v>-0.157504045</v>
       </c>
       <c r="G45" s="6">
@@ -2540,7 +2537,7 @@
       <c r="E46" s="8">
         <v>-0.48170317</v>
       </c>
-      <c r="F46" s="11">
+      <c r="F46" s="10">
         <v>-0.178168155</v>
       </c>
       <c r="G46" s="6">
@@ -2569,7 +2566,7 @@
       <c r="E47" s="8">
         <v>-0.590169861</v>
       </c>
-      <c r="F47" s="11">
+      <c r="F47" s="10">
         <v>-0.200502346</v>
       </c>
       <c r="G47" s="6">
@@ -2598,7 +2595,7 @@
       <c r="E48" s="8">
         <v>-0.630350609</v>
       </c>
-      <c r="F48" s="11">
+      <c r="F48" s="10">
         <v>-0.219682468</v>
       </c>
       <c r="G48" s="6">
@@ -2627,7 +2624,7 @@
       <c r="E49" s="8">
         <v>-0.611177537</v>
       </c>
-      <c r="F49" s="11">
+      <c r="F49" s="10">
         <v>-0.234039298</v>
       </c>
       <c r="G49" s="6">
@@ -2656,7 +2653,7 @@
       <c r="E50" s="8">
         <v>-0.548312147</v>
       </c>
-      <c r="F50" s="11">
+      <c r="F50" s="10">
         <v>-0.245925221</v>
       </c>
       <c r="G50" s="6">
@@ -2685,7 +2682,7 @@
       <c r="E51" s="8">
         <v>-0.461044984</v>
       </c>
-      <c r="F51" s="11">
+      <c r="F51" s="10">
         <v>-0.258770966</v>
       </c>
       <c r="G51" s="6">
@@ -2714,7 +2711,7 @@
       <c r="E52" s="8">
         <v>-0.364519599</v>
       </c>
-      <c r="F52" s="11">
+      <c r="F52" s="10">
         <v>-0.273941725</v>
       </c>
       <c r="G52" s="6">
@@ -2743,7 +2740,7 @@
       <c r="E53" s="8">
         <v>-0.267640082</v>
       </c>
-      <c r="F53" s="11">
+      <c r="F53" s="10">
         <v>-0.29026823</v>
       </c>
       <c r="G53" s="6">
@@ -2772,7 +2769,7 @@
       <c r="E54" s="8">
         <v>-0.173133647</v>
       </c>
-      <c r="F54" s="11">
+      <c r="F54" s="10">
         <v>-0.305652739</v>
       </c>
       <c r="G54" s="6">
@@ -2801,7 +2798,7 @@
       <c r="E55" s="8">
         <v>-0.079437751</v>
       </c>
-      <c r="F55" s="11">
+      <c r="F55" s="10">
         <v>-0.318061469</v>
       </c>
       <c r="G55" s="6">
@@ -2830,7 +2827,7 @@
       <c r="E56" s="8">
         <v>0.016572569</v>
       </c>
-      <c r="F56" s="11">
+      <c r="F56" s="10">
         <v>-0.325845643</v>
       </c>
       <c r="G56" s="6">
@@ -2859,7 +2856,7 @@
       <c r="E57" s="8">
         <v>0.11926548</v>
       </c>
-      <c r="F57" s="11">
+      <c r="F57" s="10">
         <v>-0.327796199</v>
       </c>
       <c r="G57" s="6">
@@ -2888,7 +2885,7 @@
       <c r="E58" s="8">
         <v>0.231289127</v>
       </c>
-      <c r="F58" s="11">
+      <c r="F58" s="10">
         <v>-0.323387445</v>
       </c>
       <c r="G58" s="6">
@@ -2917,7 +2914,7 @@
       <c r="E59" s="8">
         <v>0.352945067</v>
       </c>
-      <c r="F59" s="11">
+      <c r="F59" s="10">
         <v>-0.312886203</v>
       </c>
       <c r="G59" s="6">
@@ -2946,7 +2943,7 @@
       <c r="E60" s="8">
         <v>0.477975118</v>
       </c>
-      <c r="F60" s="11">
+      <c r="F60" s="10">
         <v>-0.297273884</v>
       </c>
       <c r="G60" s="6">
@@ -2975,7 +2972,7 @@
       <c r="E61" s="8">
         <v>0.592422987</v>
       </c>
-      <c r="F61" s="11">
+      <c r="F61" s="10">
         <v>-0.27788477</v>
       </c>
       <c r="G61" s="6">
@@ -3004,7 +3001,7 @@
       <c r="E62" s="8">
         <v>0.67403297</v>
       </c>
-      <c r="F62" s="11">
+      <c r="F62" s="10">
         <v>-0.256028991</v>
       </c>
       <c r="G62" s="6">
@@ -3033,7 +3030,7 @@
       <c r="E63" s="8">
         <v>0.699252385</v>
       </c>
-      <c r="F63" s="11">
+      <c r="F63" s="10">
         <v>-0.232615365</v>
       </c>
       <c r="G63" s="6">
@@ -3062,7 +3059,7 @@
       <c r="E64" s="8">
         <v>0.650932699</v>
       </c>
-      <c r="F64" s="11">
+      <c r="F64" s="10">
         <v>-0.208176421</v>
       </c>
       <c r="G64" s="6">
@@ -3091,7 +3088,7 @@
       <c r="E65" s="8">
         <v>0.524390761</v>
       </c>
-      <c r="F65" s="11">
+      <c r="F65" s="10">
         <v>-0.183467768</v>
       </c>
       <c r="G65" s="6">
@@ -3120,7 +3117,7 @@
       <c r="E66" s="8">
         <v>0.328647522</v>
       </c>
-      <c r="F66" s="11">
+      <c r="F66" s="10">
         <v>-0.16040262</v>
       </c>
       <c r="G66" s="6">
@@ -3149,7 +3146,7 @@
       <c r="E67" s="8">
         <v>0.087203264</v>
       </c>
-      <c r="F67" s="11">
+      <c r="F67" s="10">
         <v>-0.142494406</v>
       </c>
       <c r="G67" s="6">
@@ -3178,7 +3175,7 @@
       <c r="E68" s="8">
         <v>-0.163335575</v>
       </c>
-      <c r="F68" s="11">
+      <c r="F68" s="10">
         <v>-0.133990889</v>
       </c>
       <c r="G68" s="6">
@@ -3207,7 +3204,7 @@
       <c r="E69" s="8">
         <v>-0.384118264</v>
       </c>
-      <c r="F69" s="11">
+      <c r="F69" s="10">
         <v>-0.137928752</v>
       </c>
       <c r="G69" s="6">
@@ -3236,7 +3233,7 @@
       <c r="E70" s="8">
         <v>-0.546160627</v>
       </c>
-      <c r="F70" s="11">
+      <c r="F70" s="10">
         <v>-0.153940047</v>
       </c>
       <c r="G70" s="6">
@@ -3265,7 +3262,7 @@
       <c r="E71" s="8">
         <v>-0.633928011</v>
       </c>
-      <c r="F71" s="11">
+      <c r="F71" s="10">
         <v>-0.177790062</v>
       </c>
       <c r="G71" s="6">
@@ -3294,7 +3291,7 @@
       <c r="E72" s="8">
         <v>-0.645633806</v>
       </c>
-      <c r="F72" s="11">
+      <c r="F72" s="10">
         <v>-0.204015366</v>
       </c>
       <c r="G72" s="6">
@@ -3323,7 +3320,7 @@
       <c r="E73" s="8">
         <v>-0.589669009</v>
       </c>
-      <c r="F73" s="11">
+      <c r="F73" s="10">
         <v>-0.228928804</v>
       </c>
       <c r="G73" s="6">
@@ -3352,7 +3349,7 @@
       <c r="E74" s="8">
         <v>-0.483414813</v>
       </c>
-      <c r="F74" s="11">
+      <c r="F74" s="10">
         <v>-0.251220693</v>
       </c>
       <c r="G74" s="6">
@@ -3381,7 +3378,7 @@
       <c r="E75" s="8">
         <v>-0.348981066</v>
       </c>
-      <c r="F75" s="11">
+      <c r="F75" s="10">
         <v>-0.270990445</v>
       </c>
       <c r="G75" s="6">
@@ -3410,7 +3407,7 @@
       <c r="E76" s="8">
         <v>-0.202994857</v>
       </c>
-      <c r="F76" s="11">
+      <c r="F76" s="10">
         <v>-0.287859184</v>
       </c>
       <c r="G76" s="6">
@@ -3439,7 +3436,7 @@
       <c r="E77" s="8">
         <v>-0.056270022</v>
       </c>
-      <c r="F77" s="11">
+      <c r="F77" s="10">
         <v>-0.300724684</v>
       </c>
       <c r="G77" s="6">
@@ -3468,7 +3465,7 @@
       <c r="E78" s="8">
         <v>0.088605963</v>
       </c>
-      <c r="F78" s="11">
+      <c r="F78" s="10">
         <v>-0.308404033</v>
       </c>
       <c r="G78" s="6">
@@ -3497,7 +3494,7 @@
       <c r="E79" s="8">
         <v>0.229486703</v>
       </c>
-      <c r="F79" s="11">
+      <c r="F79" s="10">
         <v>-0.310198623</v>
       </c>
       <c r="G79" s="6">
@@ -3526,7 +3523,7 @@
       <c r="E80" s="8">
         <v>0.363233112</v>
       </c>
-      <c r="F80" s="11">
+      <c r="F80" s="10">
         <v>-0.305988171</v>
       </c>
       <c r="G80" s="6">
@@ -3555,7 +3552,7 @@
       <c r="E81" s="8">
         <v>0.479606712</v>
       </c>
-      <c r="F81" s="11">
+      <c r="F81" s="10">
         <v>-0.296045846</v>
       </c>
       <c r="G81" s="6">
@@ -3584,7 +3581,7 @@
       <c r="E82" s="8">
         <v>0.562164146</v>
       </c>
-      <c r="F82" s="11">
+      <c r="F82" s="10">
         <v>-0.280833103</v>
       </c>
       <c r="G82" s="6">
@@ -3613,7 +3610,7 @@
       <c r="E83" s="8">
         <v>0.591443778</v>
       </c>
-      <c r="F83" s="11">
+      <c r="F83" s="10">
         <v>-0.260716128</v>
       </c>
       <c r="G83" s="6">
@@ -3642,7 +3639,7 @@
       <c r="E84" s="8">
         <v>0.553625367</v>
       </c>
-      <c r="F84" s="11">
+      <c r="F84" s="10">
         <v>-0.236033754</v>
       </c>
       <c r="G84" s="6">
@@ -3671,7 +3668,7 @@
       <c r="E85" s="8">
         <v>0.448108693</v>
       </c>
-      <c r="F85" s="11">
+      <c r="F85" s="10">
         <v>-0.207618778</v>
       </c>
       <c r="G85" s="6">
@@ -3700,7 +3697,7 @@
       <c r="E86" s="8">
         <v>0.289088795</v>
       </c>
-      <c r="F86" s="11">
+      <c r="F86" s="10">
         <v>-0.178030766</v>
       </c>
       <c r="G86" s="6">
@@ -3729,7 +3726,7 @@
       <c r="E87" s="8">
         <v>0.101615818</v>
       </c>
-      <c r="F87" s="11">
+      <c r="F87" s="10">
         <v>-0.151987019</v>
       </c>
       <c r="G87" s="6">
@@ -3758,7 +3755,7 @@
       <c r="E88" s="8">
         <v>-0.087388014</v>
       </c>
-      <c r="F88" s="11">
+      <c r="F88" s="10">
         <v>-0.135194617</v>
       </c>
       <c r="G88" s="6">
@@ -3787,7 +3784,7 @@
       <c r="E89" s="8">
         <v>-0.255091222</v>
       </c>
-      <c r="F89" s="11">
+      <c r="F89" s="10">
         <v>-0.131827221</v>
       </c>
       <c r="G89" s="6">
@@ -3816,7 +3813,7 @@
       <c r="E90" s="8">
         <v>-0.38393508</v>
       </c>
-      <c r="F90" s="11">
+      <c r="F90" s="10">
         <v>-0.142559116</v>
       </c>
       <c r="G90" s="6">
@@ -3845,7 +3842,7 @@
       <c r="E91" s="8">
         <v>-0.461121227</v>
       </c>
-      <c r="F91" s="11">
+      <c r="F91" s="10">
         <v>-0.164553459</v>
       </c>
       <c r="G91" s="6">
@@ -3874,7 +3871,7 @@
       <c r="E92" s="8">
         <v>-0.479589523</v>
       </c>
-      <c r="F92" s="11">
+      <c r="F92" s="10">
         <v>-0.192754638</v>
       </c>
       <c r="G92" s="6">
@@ -3903,7 +3900,7 @@
       <c r="E93" s="8">
         <v>-0.440404481</v>
       </c>
-      <c r="F93" s="11">
+      <c r="F93" s="10">
         <v>-0.221639791</v>
       </c>
       <c r="G93" s="6">
@@ -3932,7 +3929,7 @@
       <c r="E94" s="8">
         <v>-0.353341992</v>
       </c>
-      <c r="F94" s="11">
+      <c r="F94" s="10">
         <v>-0.246976565</v>
       </c>
       <c r="G94" s="6">
@@ -3961,7 +3958,7 @@
       <c r="E95" s="8">
         <v>-0.23385763</v>
       </c>
-      <c r="F95" s="11">
+      <c r="F95" s="10">
         <v>-0.266629946</v>
       </c>
       <c r="G95" s="6">
@@ -3990,7 +3987,7 @@
       <c r="E96" s="8">
         <v>-0.09849524</v>
       </c>
-      <c r="F96" s="11">
+      <c r="F96" s="10">
         <v>-0.28000446</v>
       </c>
       <c r="G96" s="6">
@@ -4019,7 +4016,7 @@
       <c r="E97" s="8">
         <v>0.038721476</v>
       </c>
-      <c r="F97" s="11">
+      <c r="F97" s="10">
         <v>-0.287014415</v>
       </c>
       <c r="G97" s="6">
@@ -4048,7 +4045,7 @@
       <c r="E98" s="8">
         <v>0.166390791</v>
       </c>
-      <c r="F98" s="11">
+      <c r="F98" s="10">
         <v>-0.287634176</v>
       </c>
       <c r="G98" s="6">
@@ -4077,7 +4074,7 @@
       <c r="E99" s="8">
         <v>0.274006344</v>
       </c>
-      <c r="F99" s="11">
+      <c r="F99" s="10">
         <v>-0.282049423</v>
       </c>
       <c r="G99" s="6">
@@ -4106,7 +4103,7 @@
       <c r="E100" s="8">
         <v>0.350783294</v>
       </c>
-      <c r="F100" s="11">
+      <c r="F100" s="10">
         <v>-0.270817336</v>
       </c>
       <c r="G100" s="6">
@@ -4135,7 +4132,7 @@
       <c r="E101" s="8">
         <v>0.386727563</v>
       </c>
-      <c r="F101" s="11">
+      <c r="F101" s="10">
         <v>-0.254847099</v>
       </c>
       <c r="G101" s="6">
@@ -4164,7 +4161,7 @@
       <c r="E102" s="8">
         <v>0.375728137</v>
       </c>
-      <c r="F102" s="11">
+      <c r="F102" s="10">
         <v>-0.23534788</v>
       </c>
       <c r="G102" s="6">
@@ -4193,7 +4190,7 @@
       <c r="E103" s="8">
         <v>0.318459205</v>
       </c>
-      <c r="F103" s="11">
+      <c r="F103" s="10">
         <v>-0.213975146</v>
       </c>
       <c r="G103" s="6">
@@ -4222,7 +4219,7 @@
       <c r="E104" s="8">
         <v>0.22331465</v>
       </c>
-      <c r="F104" s="11">
+      <c r="F104" s="10">
         <v>-0.193061565</v>
       </c>
       <c r="G104" s="6">
@@ -4251,7 +4248,7 @@
       <c r="E105" s="8">
         <v>0.104551064</v>
       </c>
-      <c r="F105" s="11">
+      <c r="F105" s="10">
         <v>-0.175587814</v>
       </c>
       <c r="G105" s="6">
@@ -4280,7 +4277,7 @@
       <c r="E106" s="8">
         <v>-0.020947549</v>
       </c>
-      <c r="F106" s="11">
+      <c r="F106" s="10">
         <v>-0.164582992</v>
       </c>
       <c r="G106" s="6">
@@ -4309,7 +4306,7 @@
       <c r="E107" s="8">
         <v>-0.136679812</v>
       </c>
-      <c r="F107" s="11">
+      <c r="F107" s="10">
         <v>-0.162122493</v>
       </c>
       <c r="G107" s="6">
@@ -4338,7 +4335,7 @@
       <c r="E108" s="8">
         <v>-0.228419804</v>
       </c>
-      <c r="F108" s="11">
+      <c r="F108" s="10">
         <v>-0.168516018</v>
       </c>
       <c r="G108" s="6">
@@ -4367,7 +4364,7 @@
       <c r="E109" s="8">
         <v>-0.285475625</v>
       </c>
-      <c r="F109" s="11">
+      <c r="F109" s="10">
         <v>-0.182141918</v>
       </c>
       <c r="G109" s="6">
@@ -4396,7 +4393,7 @@
       <c r="E110" s="8">
         <v>-0.302021978</v>
       </c>
-      <c r="F110" s="11">
+      <c r="F110" s="10">
         <v>-0.199983427</v>
       </c>
       <c r="G110" s="6">
@@ -4425,7 +4422,7 @@
       <c r="E111" s="8">
         <v>-0.27808103</v>
       </c>
-      <c r="F111" s="11">
+      <c r="F111" s="10">
         <v>-0.218582901</v>
       </c>
       <c r="G111" s="6">
@@ -4454,7 +4451,7 @@
       <c r="E112" s="8">
         <v>-0.219490276</v>
       </c>
-      <c r="F112" s="11">
+      <c r="F112" s="10">
         <v>-0.235004652</v>
       </c>
       <c r="G112" s="6">
@@ -4483,7 +4480,7 @@
       <c r="E113" s="8">
         <v>-0.136450899</v>
       </c>
-      <c r="F113" s="11">
+      <c r="F113" s="10">
         <v>-0.247387304</v>
       </c>
       <c r="G113" s="6">
@@ -4512,7 +4509,7 @@
       <c r="E114" s="8">
         <v>-0.041241562</v>
       </c>
-      <c r="F114" s="11">
+      <c r="F114" s="10">
         <v>-0.254898289</v>
       </c>
       <c r="G114" s="6">
@@ -4541,7 +4538,7 @@
       <c r="E115" s="8">
         <v>0.05372075</v>
       </c>
-      <c r="F115" s="11">
+      <c r="F115" s="10">
         <v>-0.257384072</v>
       </c>
       <c r="G115" s="6">
@@ -4570,7 +4567,7 @@
       <c r="E116" s="8">
         <v>0.137069338</v>
       </c>
-      <c r="F116" s="11">
+      <c r="F116" s="10">
         <v>-0.255091939</v>
       </c>
       <c r="G116" s="6">
@@ -4599,7 +4596,7 @@
       <c r="E117" s="8">
         <v>0.199062007</v>
       </c>
-      <c r="F117" s="11">
+      <c r="F117" s="10">
         <v>-0.248590126</v>
       </c>
       <c r="G117" s="6">
@@ -4628,7 +4625,7 @@
       <c r="E118" s="8">
         <v>0.232362426</v>
       </c>
-      <c r="F118" s="11">
+      <c r="F118" s="10">
         <v>-0.238776113</v>
       </c>
       <c r="G118" s="6">
@@ -4657,7 +4654,7 @@
       <c r="E119" s="8">
         <v>0.233075441</v>
       </c>
-      <c r="F119" s="11">
+      <c r="F119" s="10">
         <v>-0.226866556</v>
       </c>
       <c r="G119" s="6">
@@ -4671,151 +4668,151 @@
       </c>
     </row>
     <row r="120" spans="1:9">
-      <c r="A120" s="12"/>
-      <c r="B120" s="12"/>
-      <c r="G120" s="12"/>
-      <c r="H120" s="12"/>
-      <c r="I120" s="12"/>
+      <c r="A120" s="11"/>
+      <c r="B120" s="11"/>
+      <c r="G120" s="11"/>
+      <c r="H120" s="11"/>
+      <c r="I120" s="11"/>
     </row>
     <row r="121" spans="1:9">
-      <c r="A121" s="12"/>
-      <c r="B121" s="12"/>
-      <c r="G121" s="12"/>
-      <c r="H121" s="12"/>
-      <c r="I121" s="12"/>
+      <c r="A121" s="11"/>
+      <c r="B121" s="11"/>
+      <c r="G121" s="11"/>
+      <c r="H121" s="11"/>
+      <c r="I121" s="11"/>
     </row>
     <row r="122" spans="1:9">
-      <c r="A122" s="12"/>
-      <c r="B122" s="12"/>
-      <c r="G122" s="12"/>
-      <c r="H122" s="12"/>
-      <c r="I122" s="12"/>
+      <c r="A122" s="11"/>
+      <c r="B122" s="11"/>
+      <c r="G122" s="11"/>
+      <c r="H122" s="11"/>
+      <c r="I122" s="11"/>
     </row>
     <row r="123" spans="1:9">
-      <c r="A123" s="12"/>
-      <c r="B123" s="12"/>
-      <c r="G123" s="12"/>
-      <c r="H123" s="12"/>
-      <c r="I123" s="12"/>
+      <c r="A123" s="11"/>
+      <c r="B123" s="11"/>
+      <c r="G123" s="11"/>
+      <c r="H123" s="11"/>
+      <c r="I123" s="11"/>
     </row>
     <row r="124" spans="1:9">
-      <c r="A124" s="12"/>
-      <c r="B124" s="12"/>
-      <c r="G124" s="12"/>
-      <c r="H124" s="12"/>
-      <c r="I124" s="12"/>
+      <c r="A124" s="11"/>
+      <c r="B124" s="11"/>
+      <c r="G124" s="11"/>
+      <c r="H124" s="11"/>
+      <c r="I124" s="11"/>
     </row>
     <row r="125" spans="1:9">
-      <c r="A125" s="12"/>
-      <c r="B125" s="12"/>
-      <c r="G125" s="12"/>
-      <c r="H125" s="12"/>
-      <c r="I125" s="12"/>
+      <c r="A125" s="11"/>
+      <c r="B125" s="11"/>
+      <c r="G125" s="11"/>
+      <c r="H125" s="11"/>
+      <c r="I125" s="11"/>
     </row>
     <row r="126" spans="1:9">
-      <c r="A126" s="12"/>
-      <c r="B126" s="12"/>
-      <c r="G126" s="12"/>
-      <c r="H126" s="12"/>
-      <c r="I126" s="12"/>
+      <c r="A126" s="11"/>
+      <c r="B126" s="11"/>
+      <c r="G126" s="11"/>
+      <c r="H126" s="11"/>
+      <c r="I126" s="11"/>
     </row>
     <row r="127" spans="1:9">
-      <c r="A127" s="12"/>
-      <c r="B127" s="12"/>
-      <c r="G127" s="12"/>
-      <c r="H127" s="12"/>
-      <c r="I127" s="12"/>
+      <c r="A127" s="11"/>
+      <c r="B127" s="11"/>
+      <c r="G127" s="11"/>
+      <c r="H127" s="11"/>
+      <c r="I127" s="11"/>
     </row>
     <row r="128" spans="1:9">
-      <c r="A128" s="12"/>
-      <c r="B128" s="12"/>
-      <c r="G128" s="12"/>
-      <c r="H128" s="12"/>
-      <c r="I128" s="12"/>
+      <c r="A128" s="11"/>
+      <c r="B128" s="11"/>
+      <c r="G128" s="11"/>
+      <c r="H128" s="11"/>
+      <c r="I128" s="11"/>
     </row>
     <row r="129" spans="1:9">
-      <c r="A129" s="12"/>
-      <c r="B129" s="12"/>
-      <c r="G129" s="12"/>
-      <c r="H129" s="12"/>
-      <c r="I129" s="12"/>
+      <c r="A129" s="11"/>
+      <c r="B129" s="11"/>
+      <c r="G129" s="11"/>
+      <c r="H129" s="11"/>
+      <c r="I129" s="11"/>
     </row>
     <row r="130" spans="1:9">
-      <c r="A130" s="12"/>
-      <c r="B130" s="12"/>
-      <c r="G130" s="12"/>
-      <c r="H130" s="12"/>
-      <c r="I130" s="12"/>
+      <c r="A130" s="11"/>
+      <c r="B130" s="11"/>
+      <c r="G130" s="11"/>
+      <c r="H130" s="11"/>
+      <c r="I130" s="11"/>
     </row>
     <row r="131" spans="1:9">
-      <c r="A131" s="12"/>
-      <c r="B131" s="12"/>
-      <c r="G131" s="12"/>
-      <c r="H131" s="12"/>
-      <c r="I131" s="12"/>
+      <c r="A131" s="11"/>
+      <c r="B131" s="11"/>
+      <c r="G131" s="11"/>
+      <c r="H131" s="11"/>
+      <c r="I131" s="11"/>
     </row>
     <row r="132" spans="1:9">
-      <c r="A132" s="12"/>
-      <c r="B132" s="12"/>
-      <c r="G132" s="12"/>
-      <c r="H132" s="12"/>
-      <c r="I132" s="12"/>
+      <c r="A132" s="11"/>
+      <c r="B132" s="11"/>
+      <c r="G132" s="11"/>
+      <c r="H132" s="11"/>
+      <c r="I132" s="11"/>
     </row>
     <row r="133" spans="1:9">
-      <c r="A133" s="12"/>
-      <c r="B133" s="12"/>
-      <c r="G133" s="12"/>
-      <c r="H133" s="12"/>
-      <c r="I133" s="12"/>
+      <c r="A133" s="11"/>
+      <c r="B133" s="11"/>
+      <c r="G133" s="11"/>
+      <c r="H133" s="11"/>
+      <c r="I133" s="11"/>
     </row>
     <row r="134" spans="1:9">
-      <c r="A134" s="12"/>
-      <c r="B134" s="12"/>
-      <c r="G134" s="12"/>
-      <c r="H134" s="12"/>
-      <c r="I134" s="12"/>
+      <c r="A134" s="11"/>
+      <c r="B134" s="11"/>
+      <c r="G134" s="11"/>
+      <c r="H134" s="11"/>
+      <c r="I134" s="11"/>
     </row>
     <row r="135" spans="1:9">
-      <c r="A135" s="12"/>
-      <c r="B135" s="12"/>
-      <c r="G135" s="12"/>
-      <c r="H135" s="12"/>
-      <c r="I135" s="12"/>
+      <c r="A135" s="11"/>
+      <c r="B135" s="11"/>
+      <c r="G135" s="11"/>
+      <c r="H135" s="11"/>
+      <c r="I135" s="11"/>
     </row>
     <row r="136" spans="1:9">
-      <c r="A136" s="12"/>
-      <c r="B136" s="12"/>
-      <c r="G136" s="12"/>
-      <c r="H136" s="12"/>
-      <c r="I136" s="12"/>
+      <c r="A136" s="11"/>
+      <c r="B136" s="11"/>
+      <c r="G136" s="11"/>
+      <c r="H136" s="11"/>
+      <c r="I136" s="11"/>
     </row>
     <row r="137" spans="1:9">
-      <c r="A137" s="12"/>
-      <c r="B137" s="12"/>
-      <c r="G137" s="12"/>
-      <c r="H137" s="12"/>
-      <c r="I137" s="12"/>
+      <c r="A137" s="11"/>
+      <c r="B137" s="11"/>
+      <c r="G137" s="11"/>
+      <c r="H137" s="11"/>
+      <c r="I137" s="11"/>
     </row>
     <row r="138" spans="1:9">
-      <c r="A138" s="12"/>
-      <c r="B138" s="12"/>
-      <c r="G138" s="12"/>
-      <c r="H138" s="12"/>
-      <c r="I138" s="12"/>
+      <c r="A138" s="11"/>
+      <c r="B138" s="11"/>
+      <c r="G138" s="11"/>
+      <c r="H138" s="11"/>
+      <c r="I138" s="11"/>
     </row>
     <row r="139" spans="1:9">
-      <c r="A139" s="12"/>
-      <c r="B139" s="12"/>
-      <c r="G139" s="12"/>
-      <c r="H139" s="12"/>
-      <c r="I139" s="12"/>
+      <c r="A139" s="11"/>
+      <c r="B139" s="11"/>
+      <c r="G139" s="11"/>
+      <c r="H139" s="11"/>
+      <c r="I139" s="11"/>
     </row>
     <row r="140" spans="1:9">
-      <c r="A140" s="12"/>
-      <c r="B140" s="12"/>
-      <c r="G140" s="12"/>
-      <c r="H140" s="12"/>
-      <c r="I140" s="12"/>
+      <c r="A140" s="11"/>
+      <c r="B140" s="11"/>
+      <c r="G140" s="11"/>
+      <c r="H140" s="11"/>
+      <c r="I140" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>